<commit_message>
small changes in documentation, requirements added, readme almost completed
</commit_message>
<xml_diff>
--- a/requirements/Requirements - conceptual mapping-csv.xlsx
+++ b/requirements/Requirements - conceptual mapping-csv.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aiglesias/GitHub/EBOCA-Evidences/requirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3A6055A-3598-AD40-9F37-97B214AEC488}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{956BEAC8-DAA5-7E4C-B6F0-29F651F3942B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="18860" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Identifier</t>
   </si>
@@ -44,6 +44,78 @@
   </si>
   <si>
     <t>Extracted from</t>
+  </si>
+  <si>
+    <t>eboca-ev1</t>
+  </si>
+  <si>
+    <t>An association can have an evidence</t>
+  </si>
+  <si>
+    <t>Evidences may be inferred or documented</t>
+  </si>
+  <si>
+    <t>Evidences are extracted from texts</t>
+  </si>
+  <si>
+    <t>Texts and its parts can be uniquely identified</t>
+  </si>
+  <si>
+    <t>Evidences have a date of creation and update</t>
+  </si>
+  <si>
+    <t>Evidences may be created with software</t>
+  </si>
+  <si>
+    <t>eboca-ev2</t>
+  </si>
+  <si>
+    <t>eboca-ev3</t>
+  </si>
+  <si>
+    <t>eboca-ev4</t>
+  </si>
+  <si>
+    <t>eboca-ev5</t>
+  </si>
+  <si>
+    <t>eboca-ev6</t>
+  </si>
+  <si>
+    <t>Themis test</t>
+  </si>
+  <si>
+    <t>sio:SIO_000897 sio:SIO000772 Evidence ;</t>
+  </si>
+  <si>
+    <t>obo:ECO_0007672 subclassof obo:ECO_0000000 ;
+obo:ECO_0006151 subclassof obo:ECO_0000000 ;
+Evidence subclassof obo:ECO_0000000 ;</t>
+  </si>
+  <si>
+    <t>Evidence pav:derivedFrom doco:Paragraph ;
+fabio:Expression frbr:part doco:Paragraph ;</t>
+  </si>
+  <si>
+    <t>fabio:Expression dc:identifier rdf:Literal ;
+doco:Paragraph dc:identifier rdf:Literal ;</t>
+  </si>
+  <si>
+    <t>Evidence pav:createdOn xsd:date ;
+Evidence pav:lastUpdatedOn xsd:dateTime ;</t>
+  </si>
+  <si>
+    <t>Evidence may be created with a confidence score</t>
+  </si>
+  <si>
+    <t>eboca-ev7</t>
+  </si>
+  <si>
+    <t>sio:SIO_000897 sio:SIO000772 Evidence ;
+sio:SIO_000897 pav:createdWith dc:Software ;</t>
+  </si>
+  <si>
+    <t>Evidence score xsd:float ;</t>
   </si>
 </sst>
 </file>
@@ -453,22 +525,23 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D1041"/>
+  <dimension ref="A1:E1041"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="10.1640625" customWidth="1"/>
     <col min="2" max="2" width="40" customWidth="1"/>
-    <col min="3" max="3" width="62.1640625" customWidth="1"/>
-    <col min="4" max="4" width="36.5" customWidth="1"/>
+    <col min="3" max="3" width="6.5" customWidth="1"/>
+    <col min="4" max="4" width="5.5" customWidth="1"/>
+    <col min="5" max="5" width="47.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="14">
+    <row r="1" spans="1:5" ht="14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -481,71 +554,132 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="13">
-      <c r="A2" s="14"/>
-      <c r="B2" s="15"/>
+      <c r="E1" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="14">
+      <c r="A2" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>5</v>
+      </c>
       <c r="C2" s="15"/>
       <c r="D2" s="9"/>
-    </row>
-    <row r="3" spans="1:4" ht="13">
-      <c r="A3" s="14"/>
-      <c r="B3" s="15"/>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="41" customHeight="1">
+      <c r="A3" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>6</v>
+      </c>
       <c r="C3" s="15"/>
       <c r="D3" s="9"/>
-    </row>
-    <row r="4" spans="1:4" ht="13">
-      <c r="A4" s="14"/>
-      <c r="B4" s="15"/>
+      <c r="E3" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="28">
+      <c r="A4" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>7</v>
+      </c>
       <c r="C4" s="15"/>
       <c r="D4" s="9"/>
-    </row>
-    <row r="5" spans="1:4" ht="13">
-      <c r="A5" s="14"/>
-      <c r="B5" s="15"/>
+      <c r="E4" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="28">
+      <c r="A5" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>8</v>
+      </c>
       <c r="C5" s="15"/>
       <c r="D5" s="9"/>
-    </row>
-    <row r="6" spans="1:4" ht="13"/>
-    <row r="7" spans="1:4" ht="13"/>
-    <row r="8" spans="1:4" ht="13"/>
-    <row r="9" spans="1:4" ht="13">
+      <c r="E5" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="28">
+      <c r="A6" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="28">
+      <c r="A7" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="28">
+      <c r="A8" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="13">
       <c r="A9" s="10"/>
       <c r="B9" s="9"/>
       <c r="C9" s="13"/>
       <c r="D9" s="9"/>
     </row>
-    <row r="10" spans="1:4" ht="13">
+    <row r="10" spans="1:5" ht="13">
       <c r="A10" s="10"/>
       <c r="B10" s="11"/>
       <c r="D10" s="9"/>
     </row>
-    <row r="11" spans="1:4" ht="13">
+    <row r="11" spans="1:5" ht="13">
       <c r="A11" s="10"/>
       <c r="B11" s="9"/>
     </row>
-    <row r="12" spans="1:4" ht="13">
+    <row r="12" spans="1:5" ht="13">
       <c r="A12" s="10"/>
       <c r="B12" s="9"/>
       <c r="D12" s="9"/>
     </row>
-    <row r="13" spans="1:4" ht="13">
+    <row r="13" spans="1:5" ht="13">
       <c r="A13" s="10"/>
       <c r="B13" s="9"/>
       <c r="C13" s="13"/>
       <c r="D13" s="9"/>
     </row>
-    <row r="14" spans="1:4" ht="13">
+    <row r="14" spans="1:5" ht="13">
       <c r="A14" s="10"/>
       <c r="B14" s="12"/>
       <c r="D14" s="9"/>
     </row>
-    <row r="15" spans="1:4" ht="13">
+    <row r="15" spans="1:5" ht="13">
       <c r="A15" s="10"/>
       <c r="B15" s="11"/>
       <c r="D15" s="9"/>
     </row>
-    <row r="16" spans="1:4" ht="13">
+    <row r="16" spans="1:5" ht="13">
       <c r="A16" s="10"/>
       <c r="B16" s="11"/>
       <c r="C16" s="13"/>

</xml_diff>

<commit_message>
small fixes accordin to requirements!
</commit_message>
<xml_diff>
--- a/requirements/Requirements - conceptual mapping-csv.xlsx
+++ b/requirements/Requirements - conceptual mapping-csv.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aiglesias/GitHub/EBOCA-Evidences/requirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{956BEAC8-DAA5-7E4C-B6F0-29F651F3942B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{401164CB-E101-1F46-9ED1-38D0CCA13984}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="18860" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-31360" yWindow="-820" windowWidth="22400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
@@ -85,26 +85,6 @@
     <t>Themis test</t>
   </si>
   <si>
-    <t>sio:SIO_000897 sio:SIO000772 Evidence ;</t>
-  </si>
-  <si>
-    <t>obo:ECO_0007672 subclassof obo:ECO_0000000 ;
-obo:ECO_0006151 subclassof obo:ECO_0000000 ;
-Evidence subclassof obo:ECO_0000000 ;</t>
-  </si>
-  <si>
-    <t>Evidence pav:derivedFrom doco:Paragraph ;
-fabio:Expression frbr:part doco:Paragraph ;</t>
-  </si>
-  <si>
-    <t>fabio:Expression dc:identifier rdf:Literal ;
-doco:Paragraph dc:identifier rdf:Literal ;</t>
-  </si>
-  <si>
-    <t>Evidence pav:createdOn xsd:date ;
-Evidence pav:lastUpdatedOn xsd:dateTime ;</t>
-  </si>
-  <si>
     <t>Evidence may be created with a confidence score</t>
   </si>
   <si>
@@ -115,7 +95,27 @@
 sio:SIO_000897 pav:createdWith dc:Software ;</t>
   </si>
   <si>
-    <t>Evidence score xsd:float ;</t>
+    <t>SIO_000897 SIO000772 Evidence ;</t>
+  </si>
+  <si>
+    <t>ECO_0006151 subClassOf ECO_0000000 ;
+ECO_0007672 subClassOf ECO_0000000 ;
+Evidence subClassOf ECO_0000000 ;</t>
+  </si>
+  <si>
+    <t>Evidence createdOn dateTime ;
+Evidence lastUpdateOn dateTime ;</t>
+  </si>
+  <si>
+    <t>Evidence score float ;</t>
+  </si>
+  <si>
+    <t>Evidence derivedFrom Paragraph ;
+Expression part Paragraph ;</t>
+  </si>
+  <si>
+    <t>Expression identifier Literal ;
+Paragraph identifier Literal ;</t>
   </si>
 </sst>
 </file>
@@ -529,7 +529,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -537,11 +537,11 @@
     <col min="1" max="1" width="10.1640625" customWidth="1"/>
     <col min="2" max="2" width="40" customWidth="1"/>
     <col min="3" max="3" width="6.5" customWidth="1"/>
-    <col min="4" max="4" width="5.5" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" customWidth="1"/>
     <col min="5" max="5" width="47.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14">
+    <row r="1" spans="1:5" ht="42">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -568,7 +568,7 @@
       <c r="C2" s="15"/>
       <c r="D2" s="9"/>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="41" customHeight="1">
@@ -581,7 +581,7 @@
       <c r="C3" s="15"/>
       <c r="D3" s="9"/>
       <c r="E3" s="13" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="28">
@@ -594,7 +594,7 @@
       <c r="C4" s="15"/>
       <c r="D4" s="9"/>
       <c r="E4" s="13" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="28">
@@ -607,7 +607,7 @@
       <c r="C5" s="15"/>
       <c r="D5" s="9"/>
       <c r="E5" s="13" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="28">
@@ -618,7 +618,7 @@
         <v>9</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="28">
@@ -629,18 +629,18 @@
         <v>10</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="28">
+    <row r="8" spans="1:5" ht="13" customHeight="1">
       <c r="A8" s="14" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="13">

</xml_diff>

<commit_message>
testsuite from themis added
</commit_message>
<xml_diff>
--- a/requirements/Requirements - conceptual mapping-csv.xlsx
+++ b/requirements/Requirements - conceptual mapping-csv.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aiglesias/GitHub/EBOCA-Evidences/requirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{401164CB-E101-1F46-9ED1-38D0CCA13984}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00C070E6-8404-BE41-9CB3-65AA41A1364D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-31360" yWindow="-820" windowWidth="22400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -91,10 +91,6 @@
     <t>eboca-ev7</t>
   </si>
   <si>
-    <t>sio:SIO_000897 sio:SIO000772 Evidence ;
-sio:SIO_000897 pav:createdWith dc:Software ;</t>
-  </si>
-  <si>
     <t>SIO_000897 SIO000772 Evidence ;</t>
   </si>
   <si>
@@ -116,6 +112,10 @@
   <si>
     <t>Expression identifier Literal ;
 Paragraph identifier Literal ;</t>
+  </si>
+  <si>
+    <t>SIO_000897 SIO000772 Evidence ;
+SIO_000897 createdWith Software ;</t>
   </si>
 </sst>
 </file>
@@ -529,7 +529,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
+      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -568,7 +568,7 @@
       <c r="C2" s="15"/>
       <c r="D2" s="9"/>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="41" customHeight="1">
@@ -581,7 +581,7 @@
       <c r="C3" s="15"/>
       <c r="D3" s="9"/>
       <c r="E3" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="28">
@@ -594,7 +594,7 @@
       <c r="C4" s="15"/>
       <c r="D4" s="9"/>
       <c r="E4" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="28">
@@ -607,7 +607,7 @@
       <c r="C5" s="15"/>
       <c r="D5" s="9"/>
       <c r="E5" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="28">
@@ -618,7 +618,7 @@
         <v>9</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="28">
@@ -629,7 +629,7 @@
         <v>10</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="13" customHeight="1">
@@ -640,7 +640,7 @@
         <v>17</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="13">

</xml_diff>

<commit_message>
diagram and requirements updated
</commit_message>
<xml_diff>
--- a/requirements/Requirements - conceptual mapping-csv.xlsx
+++ b/requirements/Requirements - conceptual mapping-csv.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aiglesias/GitHub/EBOCA-Evidences/requirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00C070E6-8404-BE41-9CB3-65AA41A1364D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D76DDAF-2401-5243-BD34-DCC0EBCC69B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-31360" yWindow="-820" windowWidth="22400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Identifier</t>
   </si>
@@ -116,6 +116,24 @@
   <si>
     <t>SIO_000897 SIO000772 Evidence ;
 SIO_000897 createdWith Software ;</t>
+  </si>
+  <si>
+    <t>eboca-ev8</t>
+  </si>
+  <si>
+    <t>eboca-ev9</t>
+  </si>
+  <si>
+    <t>How many evidences of associations with chemicals has each gene?</t>
+  </si>
+  <si>
+    <t>Which associations between diseases and chemicals have more than one evidence?</t>
+  </si>
+  <si>
+    <t>SPARQL (CQ-EV1)</t>
+  </si>
+  <si>
+    <t>SPARQL (CQ-EV2)</t>
   </si>
 </sst>
 </file>
@@ -529,7 +547,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
+      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -541,7 +559,7 @@
     <col min="5" max="5" width="47.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="42">
+    <row r="1" spans="1:5" ht="28">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -643,16 +661,30 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="13">
-      <c r="A9" s="10"/>
-      <c r="B9" s="9"/>
+    <row r="9" spans="1:5" ht="26" customHeight="1">
+      <c r="A9" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>28</v>
+      </c>
       <c r="C9" s="13"/>
       <c r="D9" s="9"/>
-    </row>
-    <row r="10" spans="1:5" ht="13">
-      <c r="A10" s="10"/>
-      <c r="B10" s="11"/>
+      <c r="E9" s="13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="28">
+      <c r="A10" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>29</v>
+      </c>
       <c r="D10" s="9"/>
+      <c r="E10" s="13" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="11" spans="1:5" ht="13">
       <c r="A11" s="10"/>

</xml_diff>